<commit_message>
looks fine but I have a major bug
</commit_message>
<xml_diff>
--- a/src/xml_measurements/figure_out_the_name.xlsx
+++ b/src/xml_measurements/figure_out_the_name.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Profesori</t>
   </si>
@@ -34,21 +34,12 @@
     <t>Voluntar</t>
   </si>
   <si>
-    <t>PETRUSEL Adrian</t>
-  </si>
-  <si>
-    <t>petrusel[at]math.ubbcluj.ro</t>
-  </si>
-  <si>
     <t>da</t>
   </si>
   <si>
     <t>nu vine</t>
   </si>
   <si>
-    <t>mail</t>
-  </si>
-  <si>
     <t>Alexandra Pasca</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>dadi[at]cs.ubbcluj.ro</t>
   </si>
   <si>
-    <t>mail/f2f</t>
-  </si>
-  <si>
     <t>Alexandra Pasca/Rareș Rad</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>mircea[at]cs.ubbcluj.ro</t>
   </si>
   <si>
-    <t>mail/FB</t>
-  </si>
-  <si>
     <t>SUCIU Dan Mircea</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>IANCU Mihai</t>
   </si>
   <si>
-    <t>F2f</t>
-  </si>
-  <si>
     <t>MOGA Madalina</t>
   </si>
   <si>
@@ -244,13 +226,7 @@
     <t>Da</t>
   </si>
   <si>
-    <t>FB</t>
-  </si>
-  <si>
     <t>Szasz Paul</t>
-  </si>
-  <si>
-    <t>Mail</t>
   </si>
 </sst>
 </file>
@@ -266,12 +242,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,8 +268,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,582 +592,582 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2">
+        <v>5.43</v>
+      </c>
+      <c r="B2">
+        <v>3.21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="str">
         <f>sum(A2, B2)</f>
-        <v>0</v>
+        <v>8.64</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
         <f>sum(A3, B3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
         <f>sum(A4, B4)</f>
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
         <f>sum(A5, B5)</f>
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
         <f>sum(A6, B6)</f>
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
         <f>sum(A7, B7)</f>
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
         <f>sum(A8, B8)</f>
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
         <f>sum(A9, B9)</f>
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
         <f>sum(A10, B10)</f>
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
         <f>sum(A11, B11)</f>
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1">
         <f>sum(A12, B12)</f>
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
         <f>sum(A13, B13)</f>
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
         <f>sum(A14, B14)</f>
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1">
         <f>sum(A15, B15)</f>
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1">
         <f>sum(A16, B16)</f>
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17">
+        <v>41</v>
+      </c>
+      <c r="E17" s="1">
         <f>sum(A17, B17)</f>
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
         <f>sum(A18, B18)</f>
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1">
         <f>sum(A19, B19)</f>
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
         <f>sum(A20, B20)</f>
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1">
         <f>sum(A21, B21)</f>
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1">
         <f>sum(A22, B22)</f>
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1">
         <f>sum(A23, B23)</f>
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24">
+        <v>57</v>
+      </c>
+      <c r="E24" s="1">
         <f>sum(A24, B24)</f>
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25">
+        <v>57</v>
+      </c>
+      <c r="E25" s="1">
         <f>sum(A25, B25)</f>
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1">
         <f>sum(A26, B26)</f>
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1">
         <f>sum(A27, B27)</f>
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1">
         <f>sum(A28, B28)</f>
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29">
+        <v>69</v>
+      </c>
+      <c r="E29" s="1">
         <f>sum(A29, B29)</f>
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30">
+        <v>69</v>
+      </c>
+      <c r="E30" s="1">
         <f>sum(A30, B30)</f>
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>